<commit_message>
typos correction and combine sensitivity analysis
</commit_message>
<xml_diff>
--- a/Model_Inputs.xlsx
+++ b/Model_Inputs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Zack/Downloads/gurobi-optimization-class-tool-main-2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Zack/Downloads/gurobi-optimization-class-tool-main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C0E302-F103-A24C-80D6-3CA9C2946511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35FA5E9F-BA29-2D40-9163-688AE3C9D45A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21140" yWindow="500" windowWidth="35360" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10720" yWindow="500" windowWidth="35360" windowHeight="16880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
   <si>
     <t>Objective coefficients</t>
   </si>
@@ -58,27 +58,12 @@
     <t>Upper bound</t>
   </si>
   <si>
-    <t>B2 corresponds to variable 1, C2 corrsponds to variable 2, D2 corresponds to variable 3, etc. It cannot be left empty until the last variable.</t>
-  </si>
-  <si>
     <t>Constraints</t>
   </si>
   <si>
-    <t>Constraints are defined on the "Constraints" sheets:</t>
-  </si>
-  <si>
     <t>Inputs</t>
   </si>
   <si>
-    <t>Could be -inf, all any number(don't use "" on numbers), if empty then it is set as 0.</t>
-  </si>
-  <si>
-    <t>Could be +inf, all any number(don't use "" on numbers), if empty then it is set as +inf.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1. each row represents a constraint,</t>
-  </si>
-  <si>
     <t>2. the left side of column(constraint type) corresponds to the constraint coefficients,</t>
   </si>
   <si>
@@ -100,24 +85,12 @@
     <t>max or min.</t>
   </si>
   <si>
-    <t>All string inputs are case sensitive (use lower case for strings).</t>
-  </si>
-  <si>
     <t>Max number of inputs</t>
   </si>
   <si>
-    <t xml:space="preserve">10000 on variables, 100000 on constraints </t>
-  </si>
-  <si>
     <t>Variable Names</t>
   </si>
   <si>
-    <t>Variables</t>
-  </si>
-  <si>
-    <t>Optional, if empty, the ith variable will be defined as xi</t>
-  </si>
-  <si>
     <t>&gt;=</t>
   </si>
   <si>
@@ -146,6 +119,42 @@
   </si>
   <si>
     <t>painting_time</t>
+  </si>
+  <si>
+    <t>All string inputs are case sensitive.</t>
+  </si>
+  <si>
+    <t>10000 on variables, 100000 on constraints.</t>
+  </si>
+  <si>
+    <t>B2 corresponds to variable 1, C2 corrsponds to variable 2, D2 corresponds to variable 3, etc. If the coefficient of variable is 0, leave it as 0 instead as blank.</t>
+  </si>
+  <si>
+    <t>Optional, if empty, the ith variable will be defined as xi.</t>
+  </si>
+  <si>
+    <t>Constraints are defined on the "Constraints" area:</t>
+  </si>
+  <si>
+    <t>Could be -inf, or any number(don't use "" on numbers). If empty, then it is set as 0.</t>
+  </si>
+  <si>
+    <t>Could be +inf, or any number(don't use "" on numbers). If empty, then it is set as +inf.</t>
+  </si>
+  <si>
+    <t>Number of variables</t>
+  </si>
+  <si>
+    <t>Default is 2, more variables can be added by inserting a column to the left of the “constraint type” column.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. each row represents a constraint and the number of constraints are not limited to the size of "Constraints" area (i.e. you can add more rows below the defined area). </t>
+  </si>
+  <si>
+    <t>Run Sensitivity Analysis</t>
+  </si>
+  <si>
+    <t>1 (yes) or 0 (no)</t>
   </si>
 </sst>
 </file>
@@ -183,7 +192,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -243,11 +252,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -260,6 +278,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -596,7 +617,7 @@
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -614,24 +635,26 @@
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -653,12 +676,13 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
@@ -666,6 +690,9 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -675,13 +702,23 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
       <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>3</v>
@@ -694,7 +731,7 @@
         <v>2</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
@@ -708,13 +745,13 @@
         <v>4</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="E9" s="1">
         <v>2400</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -728,13 +765,13 @@
         <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="E10" s="1">
         <v>1000</v>
       </c>
-      <c r="F10" t="s">
-        <v>39</v>
+      <c r="F10" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -748,13 +785,13 @@
         <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="E11" s="1">
         <v>450</v>
       </c>
-      <c r="F11" t="s">
-        <v>34</v>
+      <c r="F11" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -768,66 +805,146 @@
         <v>0</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="E12" s="1">
         <v>100</v>
       </c>
-      <c r="F12" t="s">
-        <v>35</v>
+      <c r="F12" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
       <c r="K13" s="1"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
       <c r="K14" s="1"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
       <c r="K15" s="1"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -840,10 +957,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39AAF657-37C6-6C49-ACE1-D3F4FAA24ABE}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:I5"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -852,225 +969,258 @@
     <col min="2" max="2" width="36.83203125" customWidth="1"/>
     <col min="3" max="4" width="15.5" customWidth="1"/>
     <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
+      <c r="A1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
+        <v>11</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="10"/>
+        <v>19</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="11"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
+        <v>38</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="11"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="10"/>
+        <v>7</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="11"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
+        <v>0</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="7"/>
+      <c r="B12" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="7"/>
+      <c r="B13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="6"/>
-      <c r="B12" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
-      <c r="B13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
-      <c r="B14" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="7"/>
+      <c r="B15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="17">
+    <mergeCell ref="B4:I4"/>
+    <mergeCell ref="B16:I16"/>
     <mergeCell ref="B2:I2"/>
-    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="A11:A15"/>
     <mergeCell ref="A1:I1"/>
+    <mergeCell ref="B14:I14"/>
+    <mergeCell ref="B15:I15"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B9:I9"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="B10:I10"/>
+    <mergeCell ref="B12:I12"/>
     <mergeCell ref="B13:I13"/>
-    <mergeCell ref="B14:I14"/>
-    <mergeCell ref="B10:I10"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="B9:I9"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="B12:I12"/>
-    <mergeCell ref="B4:I4"/>
     <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>